<commit_message>
change preview image of lower SEMs
</commit_message>
<xml_diff>
--- a/docs/posts/2019-06-13-lower-sem-for-core-vs-traditional-orf/references/raw_sem_table.xlsx
+++ b/docs/posts/2019-06-13-lower-sem-for-core-vs-traditional-orf/references/raw_sem_table.xlsx
@@ -184,12 +184,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -204,9 +210,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,7 +497,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:C24"/>
+      <selection activeCell="F3" sqref="F3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +556,7 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>7.84</v>
       </c>
       <c r="D3">
@@ -558,7 +565,7 @@
       <c r="E3">
         <v>9.1199999999999992</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>7.84</v>
       </c>
       <c r="G3">
@@ -585,7 +592,7 @@
       <c r="E4">
         <v>9.59</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>9.59</v>
       </c>
       <c r="G4">
@@ -612,7 +619,7 @@
       <c r="E5">
         <v>10.08</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>9.6300000000000008</v>
       </c>
       <c r="G5">

</xml_diff>